<commit_message>
Updating Exam Bulk Questions Upload
</commit_message>
<xml_diff>
--- a/public/images/example.xlsx
+++ b/public/images/example.xlsx
@@ -1,29 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22413"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\New folder\htdocs\ucolledge\public\images\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49B1CA6-87EE-4343-8ABF-71376766FB8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9FE95B2-74FC-4B6C-B4ED-E3A56D67F110}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{19BF03ED-CFD9-4DF8-B7A2-489361D578AF}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,33 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>How many eyes does a monkey have?</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>what planet is the closest to the sun?</t>
-  </si>
-  <si>
-    <t>Mecury</t>
-  </si>
-  <si>
-    <t>Venus</t>
-  </si>
-  <si>
-    <t>Earth</t>
-  </si>
-  <si>
-    <t>Mars</t>
-  </si>
-  <si>
-    <t>A</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+  <si>
+    <t>Questions</t>
   </si>
   <si>
     <t>option_A</t>
@@ -72,20 +42,50 @@
     <t>option_D</t>
   </si>
   <si>
+    <t>option_E</t>
+  </si>
+  <si>
     <t>Correct_Answer</t>
+  </si>
+  <si>
+    <t>Which one is correct team name in NBA?</t>
+  </si>
+  <si>
+    <t>New York Bulls</t>
+  </si>
+  <si>
+    <t>Los Angeles Kings</t>
+  </si>
+  <si>
+    <t>Golden State Warriros</t>
+  </si>
+  <si>
+    <t>Huston Rocket</t>
+  </si>
+  <si>
+    <t>5 + 7 = ?</t>
+  </si>
+  <si>
+    <t>12 - 8 = ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,14 +108,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -423,77 +424,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BC5163-1D04-4E41-A736-C070E295D4EC}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="49.140625" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="1" max="1" width="53.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
         <v>13</v>
       </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>